<commit_message>
- Update ExcelReader and data format - Unit test for ExcelReader
</commit_message>
<xml_diff>
--- a/tests/data/ExcelRobotTest.xlsx
+++ b/tests/data/ExcelRobotTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sontt\Projects\work\opensource\robotframework-excel\tests\acceptance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sontt\Projects\work\opensource\robotframework-excel\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B7ED5F9-9743-429D-B0D1-41E58437F903}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F861CC-A881-4243-B2D0-F034051BF952}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Passed</t>
   </si>
@@ -77,15 +77,6 @@
     <t>User6</t>
   </si>
   <si>
-    <t>Favourite Colour</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
     <t>Team1</t>
   </si>
   <si>
@@ -105,12 +96,30 @@
   </si>
   <si>
     <t>Points</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Unemployment</t>
+  </si>
+  <si>
+    <t>Blank</t>
+  </si>
+  <si>
+    <t>Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -175,16 +184,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
-    <cellStyle name="Hyperlink 2" xfId="2"/>
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -519,11 +529,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -561,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,50 +614,79 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" s="3">
+        <v>30085</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>19</v>
+      <c r="C3" s="3">
+        <v>28593</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -666,18 +705,18 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>77</v>
@@ -691,7 +730,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>82</v>
@@ -705,7 +744,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>65</v>
@@ -723,7 +762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
- Implement Excel writer - Update test - Refactor code
</commit_message>
<xml_diff>
--- a/tests/data/ExcelRobotTest.xlsx
+++ b/tests/data/ExcelRobotTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sontt\Projects\work\opensource\robotframework-excel\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59430D5-2CB0-488B-BE4A-387E4142AEA8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B35F34-3EF9-4E87-B4A4-6ACD7F2454DE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Passed</t>
   </si>
@@ -120,14 +120,18 @@
   </si>
   <si>
     <t>Hour</t>
+  </si>
+  <si>
+    <t>Date Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="171" formatCode="yyyy/mm/dd\ hh:mm"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -193,12 +197,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -625,10 +630,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A1:H3"/>
+      <selection activeCell="I3" sqref="A1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,9 +642,10 @@
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -664,8 +670,11 @@
       <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -684,8 +693,11 @@
       <c r="H2" s="4">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="5">
+        <v>43102.916666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>

</xml_diff>